<commit_message>
Conducted further data analysis and trained AdaboostClassifier
</commit_message>
<xml_diff>
--- a/MasterData.xlsx
+++ b/MasterData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AnmolParande/Documents/Python/March Madness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EAFA2A-0A37-E642-9E9A-CFF136EDE3B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1D5B37-645C-C54F-BF18-4211D8D6EA7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{2622F5BA-9625-CD43-A056-F7E7AD14BF78}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{2622F5BA-9625-CD43-A056-F7E7AD14BF78}"/>
   </bookViews>
   <sheets>
     <sheet name="GameData" sheetId="1" r:id="rId1"/>
@@ -1494,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08E6FAD-90C2-D64F-A8C4-E3B0A2D39B82}">
   <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="F193" sqref="F193"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="H187" sqref="H187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4671,8 +4671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDC5CCE-88F0-F146-B1F6-7793F05CDE9F}">
   <dimension ref="A1:I354"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A217" sqref="A217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>